<commit_message>
Uji Coba migrasi device baru
</commit_message>
<xml_diff>
--- a/reference/Master ITEM v2.xlsx
+++ b/reference/Master ITEM v2.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Report Generator\lincreport\reference\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -784,17 +779,7 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="4"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1083,7 +1068,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1093,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,7 +3584,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A178 A229:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>